<commit_message>
Add POR documents for minor residents
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicroTech\IdeaProjects\mosip-data-guinea\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C86AA3B8-B931-49B7-8B2D-061E0B078B0C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FFC938-8120-4CD1-ACE0-4C0585017845}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19476" yWindow="312" windowWidth="9336" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1561" uniqueCount="34">
   <si>
     <t>apptyp_code</t>
   </si>
@@ -962,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E385"/>
+  <dimension ref="A1:E390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="F384" sqref="F384"/>
+    <sheetView tabSelected="1" topLeftCell="A362" workbookViewId="0">
+      <selection activeCell="I384" sqref="I384"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6075,13 +6075,13 @@
         <v>7</v>
       </c>
       <c r="B301">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C301" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D301" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="E301" t="s">
         <v>8</v>
@@ -6092,13 +6092,13 @@
         <v>7</v>
       </c>
       <c r="B302">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C302" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D302" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E302" t="s">
         <v>8</v>
@@ -6109,13 +6109,13 @@
         <v>7</v>
       </c>
       <c r="B303">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C303" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D303" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E303" t="s">
         <v>8</v>
@@ -6126,13 +6126,13 @@
         <v>7</v>
       </c>
       <c r="B304">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C304" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D304" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E304" t="s">
         <v>8</v>
@@ -6143,13 +6143,13 @@
         <v>7</v>
       </c>
       <c r="B305">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C305" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D305" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E305" t="s">
         <v>8</v>
@@ -6166,7 +6166,7 @@
         <v>5</v>
       </c>
       <c r="D306" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E306" t="s">
         <v>8</v>
@@ -6183,7 +6183,7 @@
         <v>5</v>
       </c>
       <c r="D307" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E307" t="s">
         <v>8</v>
@@ -6200,7 +6200,7 @@
         <v>5</v>
       </c>
       <c r="D308" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E308" t="s">
         <v>8</v>
@@ -6217,7 +6217,7 @@
         <v>5</v>
       </c>
       <c r="D309" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E309" t="s">
         <v>8</v>
@@ -6234,7 +6234,7 @@
         <v>5</v>
       </c>
       <c r="D310" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E310" t="s">
         <v>8</v>
@@ -6251,7 +6251,7 @@
         <v>5</v>
       </c>
       <c r="D311" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E311" t="s">
         <v>8</v>
@@ -6265,10 +6265,10 @@
         <v>15</v>
       </c>
       <c r="C312" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D312" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E312" t="s">
         <v>8</v>
@@ -6282,10 +6282,10 @@
         <v>15</v>
       </c>
       <c r="C313" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D313" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E313" t="s">
         <v>8</v>
@@ -6299,10 +6299,10 @@
         <v>15</v>
       </c>
       <c r="C314" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D314" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E314" t="s">
         <v>8</v>
@@ -6316,10 +6316,10 @@
         <v>15</v>
       </c>
       <c r="C315" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D315" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E315" t="s">
         <v>8</v>
@@ -6333,10 +6333,10 @@
         <v>15</v>
       </c>
       <c r="C316" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D316" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E316" t="s">
         <v>8</v>
@@ -6350,10 +6350,10 @@
         <v>15</v>
       </c>
       <c r="C317" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D317" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E317" t="s">
         <v>8</v>
@@ -6367,10 +6367,10 @@
         <v>15</v>
       </c>
       <c r="C318" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D318" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E318" t="s">
         <v>8</v>
@@ -6384,10 +6384,10 @@
         <v>15</v>
       </c>
       <c r="C319" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D319" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E319" t="s">
         <v>8</v>
@@ -6401,10 +6401,10 @@
         <v>15</v>
       </c>
       <c r="C320" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D320" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E320" t="s">
         <v>8</v>
@@ -6418,10 +6418,10 @@
         <v>15</v>
       </c>
       <c r="C321" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D321" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E321" t="s">
         <v>8</v>
@@ -6435,10 +6435,10 @@
         <v>15</v>
       </c>
       <c r="C322" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D322" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E322" t="s">
         <v>8</v>
@@ -6452,10 +6452,10 @@
         <v>15</v>
       </c>
       <c r="C323" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D323" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E323" t="s">
         <v>8</v>
@@ -6469,7 +6469,7 @@
         <v>15</v>
       </c>
       <c r="C324" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D324" t="s">
         <v>10</v>
@@ -6486,10 +6486,10 @@
         <v>15</v>
       </c>
       <c r="C325" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D325" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E325" t="s">
         <v>8</v>
@@ -6500,13 +6500,13 @@
         <v>7</v>
       </c>
       <c r="B326">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C326" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D326" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E326" t="s">
         <v>8</v>
@@ -6517,13 +6517,13 @@
         <v>7</v>
       </c>
       <c r="B327">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C327" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="D327" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E327" t="s">
         <v>8</v>
@@ -6534,10 +6534,10 @@
         <v>7</v>
       </c>
       <c r="B328">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C328" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D328" t="s">
         <v>6</v>
@@ -6551,13 +6551,13 @@
         <v>7</v>
       </c>
       <c r="B329">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C329" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="D329" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E329" t="s">
         <v>8</v>
@@ -6568,13 +6568,13 @@
         <v>7</v>
       </c>
       <c r="B330">
+        <v>15</v>
+      </c>
+      <c r="C330" t="s">
+        <v>28</v>
+      </c>
+      <c r="D330" t="s">
         <v>16</v>
-      </c>
-      <c r="C330" t="s">
-        <v>5</v>
-      </c>
-      <c r="D330" t="s">
-        <v>10</v>
       </c>
       <c r="E330" t="s">
         <v>8</v>
@@ -6591,7 +6591,7 @@
         <v>5</v>
       </c>
       <c r="D331" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E331" t="s">
         <v>8</v>
@@ -6608,7 +6608,7 @@
         <v>5</v>
       </c>
       <c r="D332" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E332" t="s">
         <v>8</v>
@@ -6625,7 +6625,7 @@
         <v>5</v>
       </c>
       <c r="D333" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E333" t="s">
         <v>8</v>
@@ -6642,7 +6642,7 @@
         <v>5</v>
       </c>
       <c r="D334" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E334" t="s">
         <v>8</v>
@@ -6659,7 +6659,7 @@
         <v>5</v>
       </c>
       <c r="D335" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E335" t="s">
         <v>8</v>
@@ -6676,7 +6676,7 @@
         <v>5</v>
       </c>
       <c r="D336" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E336" t="s">
         <v>8</v>
@@ -6690,10 +6690,10 @@
         <v>16</v>
       </c>
       <c r="C337" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D337" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E337" t="s">
         <v>8</v>
@@ -6707,10 +6707,10 @@
         <v>16</v>
       </c>
       <c r="C338" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D338" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E338" t="s">
         <v>8</v>
@@ -6724,10 +6724,10 @@
         <v>16</v>
       </c>
       <c r="C339" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D339" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E339" t="s">
         <v>8</v>
@@ -6741,10 +6741,10 @@
         <v>16</v>
       </c>
       <c r="C340" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D340" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E340" t="s">
         <v>8</v>
@@ -6758,10 +6758,10 @@
         <v>16</v>
       </c>
       <c r="C341" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D341" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E341" t="s">
         <v>8</v>
@@ -6775,10 +6775,10 @@
         <v>16</v>
       </c>
       <c r="C342" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D342" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E342" t="s">
         <v>8</v>
@@ -6792,10 +6792,10 @@
         <v>16</v>
       </c>
       <c r="C343" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D343" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E343" t="s">
         <v>8</v>
@@ -6809,10 +6809,10 @@
         <v>16</v>
       </c>
       <c r="C344" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D344" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E344" t="s">
         <v>8</v>
@@ -6826,10 +6826,10 @@
         <v>16</v>
       </c>
       <c r="C345" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D345" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="E345" t="s">
         <v>8</v>
@@ -6840,13 +6840,13 @@
         <v>7</v>
       </c>
       <c r="B346">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C346" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D346" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="E346" t="s">
         <v>8</v>
@@ -6857,13 +6857,13 @@
         <v>7</v>
       </c>
       <c r="B347">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C347" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D347" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E347" t="s">
         <v>8</v>
@@ -6874,13 +6874,13 @@
         <v>7</v>
       </c>
       <c r="B348">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C348" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D348" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="E348" t="s">
         <v>8</v>
@@ -6891,13 +6891,13 @@
         <v>7</v>
       </c>
       <c r="B349">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C349" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D349" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="E349" t="s">
         <v>8</v>
@@ -6908,13 +6908,13 @@
         <v>7</v>
       </c>
       <c r="B350">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C350" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D350" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E350" t="s">
         <v>8</v>
@@ -6925,7 +6925,7 @@
         <v>7</v>
       </c>
       <c r="B351">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C351" t="s">
         <v>32</v>
@@ -6942,7 +6942,7 @@
         <v>7</v>
       </c>
       <c r="B352">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C352" t="s">
         <v>32</v>
@@ -6959,7 +6959,7 @@
         <v>7</v>
       </c>
       <c r="B353">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C353" t="s">
         <v>32</v>
@@ -6976,7 +6976,7 @@
         <v>7</v>
       </c>
       <c r="B354">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C354" t="s">
         <v>32</v>
@@ -6993,7 +6993,7 @@
         <v>7</v>
       </c>
       <c r="B355">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C355" t="s">
         <v>32</v>
@@ -7010,7 +7010,7 @@
         <v>7</v>
       </c>
       <c r="B356">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C356" t="s">
         <v>32</v>
@@ -7027,7 +7027,7 @@
         <v>7</v>
       </c>
       <c r="B357">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C357" t="s">
         <v>32</v>
@@ -7044,7 +7044,7 @@
         <v>7</v>
       </c>
       <c r="B358">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C358" t="s">
         <v>32</v>
@@ -7061,7 +7061,7 @@
         <v>7</v>
       </c>
       <c r="B359">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C359" t="s">
         <v>32</v>
@@ -7078,7 +7078,7 @@
         <v>7</v>
       </c>
       <c r="B360">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C360" t="s">
         <v>32</v>
@@ -7095,7 +7095,7 @@
         <v>7</v>
       </c>
       <c r="B361">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C361" t="s">
         <v>32</v>
@@ -7112,13 +7112,13 @@
         <v>7</v>
       </c>
       <c r="B362">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C362" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D362" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="E362" t="s">
         <v>8</v>
@@ -7129,13 +7129,13 @@
         <v>7</v>
       </c>
       <c r="B363">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C363" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D363" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="E363" t="s">
         <v>8</v>
@@ -7146,13 +7146,13 @@
         <v>7</v>
       </c>
       <c r="B364">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C364" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D364" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E364" t="s">
         <v>8</v>
@@ -7163,13 +7163,13 @@
         <v>7</v>
       </c>
       <c r="B365">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C365" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D365" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E365" t="s">
         <v>8</v>
@@ -7180,13 +7180,13 @@
         <v>7</v>
       </c>
       <c r="B366">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C366" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="D366" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E366" t="s">
         <v>8</v>
@@ -7203,7 +7203,7 @@
         <v>5</v>
       </c>
       <c r="D367" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E367" t="s">
         <v>8</v>
@@ -7220,7 +7220,7 @@
         <v>5</v>
       </c>
       <c r="D368" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E368" t="s">
         <v>8</v>
@@ -7237,7 +7237,7 @@
         <v>5</v>
       </c>
       <c r="D369" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E369" t="s">
         <v>8</v>
@@ -7254,7 +7254,7 @@
         <v>5</v>
       </c>
       <c r="D370" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E370" t="s">
         <v>8</v>
@@ -7268,10 +7268,10 @@
         <v>0</v>
       </c>
       <c r="C371" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D371" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E371" t="s">
         <v>8</v>
@@ -7285,10 +7285,10 @@
         <v>0</v>
       </c>
       <c r="C372" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D372" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E372" t="s">
         <v>8</v>
@@ -7302,10 +7302,10 @@
         <v>0</v>
       </c>
       <c r="C373" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D373" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E373" t="s">
         <v>8</v>
@@ -7319,10 +7319,10 @@
         <v>0</v>
       </c>
       <c r="C374" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D374" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E374" t="s">
         <v>8</v>
@@ -7336,10 +7336,10 @@
         <v>0</v>
       </c>
       <c r="C375" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D375" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E375" t="s">
         <v>8</v>
@@ -7353,10 +7353,10 @@
         <v>0</v>
       </c>
       <c r="C376" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D376" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E376" t="s">
         <v>8</v>
@@ -7370,10 +7370,10 @@
         <v>0</v>
       </c>
       <c r="C377" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D377" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E377" t="s">
         <v>8</v>
@@ -7387,10 +7387,10 @@
         <v>0</v>
       </c>
       <c r="C378" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D378" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E378" t="s">
         <v>8</v>
@@ -7404,10 +7404,10 @@
         <v>0</v>
       </c>
       <c r="C379" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D379" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E379" t="s">
         <v>8</v>
@@ -7421,10 +7421,10 @@
         <v>0</v>
       </c>
       <c r="C380" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D380" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E380" t="s">
         <v>8</v>
@@ -7438,10 +7438,10 @@
         <v>0</v>
       </c>
       <c r="C381" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D381" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="E381" t="s">
         <v>8</v>
@@ -7455,10 +7455,10 @@
         <v>0</v>
       </c>
       <c r="C382" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D382" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E382" t="s">
         <v>8</v>
@@ -7472,7 +7472,7 @@
         <v>0</v>
       </c>
       <c r="C383" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D383" t="s">
         <v>10</v>
@@ -7489,10 +7489,10 @@
         <v>0</v>
       </c>
       <c r="C384" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D384" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E384" t="s">
         <v>8</v>
@@ -7506,12 +7506,97 @@
         <v>0</v>
       </c>
       <c r="C385" t="s">
+        <v>23</v>
+      </c>
+      <c r="D385" t="s">
+        <v>14</v>
+      </c>
+      <c r="E385" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>7</v>
+      </c>
+      <c r="B386">
+        <v>0</v>
+      </c>
+      <c r="C386" t="s">
+        <v>26</v>
+      </c>
+      <c r="D386" t="s">
+        <v>27</v>
+      </c>
+      <c r="E386" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>7</v>
+      </c>
+      <c r="B387">
+        <v>0</v>
+      </c>
+      <c r="C387" t="s">
+        <v>28</v>
+      </c>
+      <c r="D387" t="s">
+        <v>6</v>
+      </c>
+      <c r="E387" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>7</v>
+      </c>
+      <c r="B388">
+        <v>0</v>
+      </c>
+      <c r="C388" t="s">
+        <v>28</v>
+      </c>
+      <c r="D388" t="s">
+        <v>10</v>
+      </c>
+      <c r="E388" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>7</v>
+      </c>
+      <c r="B389">
+        <v>0</v>
+      </c>
+      <c r="C389" t="s">
+        <v>28</v>
+      </c>
+      <c r="D389" t="s">
+        <v>16</v>
+      </c>
+      <c r="E389" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>7</v>
+      </c>
+      <c r="B390">
+        <v>0</v>
+      </c>
+      <c r="C390" t="s">
         <v>32</v>
       </c>
-      <c r="D385" t="s">
+      <c r="D390" t="s">
         <v>33</v>
       </c>
-      <c r="E385" t="s">
+      <c r="E390" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>